<commit_message>
Add Maven configuration for Java 8 and implement HTML report export
</commit_message>
<xml_diff>
--- a/out/reporte_notas.xlsx
+++ b/out/reporte_notas.xlsx
@@ -22,7 +22,12 @@
   <si>
     <r>
       <t xml:space="preserve">BANCA DIGITAL
-DETALLE DE NOTAS TRASNMITIDAS</t>
+DETALLE DE NOTAS TRANSNMITIDAS</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">FECHA DE IMPRESIÓN: 25/09/20252</t>
     </r>
   </si>
   <si>
@@ -91,6 +96,11 @@
   <si>
     <r>
       <t xml:space="preserve">$20,000.00</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">789 - RQWER </t>
     </r>
   </si>
   <si>
@@ -269,9 +279,9 @@
     <col min="2" max="2" customWidth="1" width="5.0"/>
     <col min="3" max="3" customWidth="1" width="18.166666"/>
     <col min="4" max="4" customWidth="1" width="10.166667"/>
-    <col min="5" max="5" customWidth="1" width="8.333333"/>
-    <col min="6" max="6" customWidth="1" width="3.3333333"/>
-    <col min="7" max="7" customWidth="1" width="23.333334"/>
+    <col min="5" max="5" customWidth="1" width="11.666667"/>
+    <col min="6" max="6" customWidth="1" width="11.666667"/>
+    <col min="7" max="7" customWidth="1" width="11.666667"/>
     <col min="8" max="8" customWidth="1" width="15.0"/>
     <col min="9" max="9" customWidth="1" width="6.6666665"/>
   </cols>
@@ -302,1292 +312,1374 @@
       <c r="H2" s="3" t="s"/>
       <c r="I2" s="2" t="s"/>
     </row>
-    <row r="3" customHeight="1" ht="60">
-      <c r="A3" s="4" t="s">
+    <row r="3" customHeight="1" ht="3">
+      <c r="A3" s="2" t="s"/>
+      <c r="B3" s="2" t="s"/>
+      <c r="C3" s="2" t="s"/>
+      <c r="D3" s="2" t="s"/>
+      <c r="E3" s="2" t="s"/>
+      <c r="F3" s="2" t="s"/>
+      <c r="G3" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="4" t="s"/>
-      <c r="C3" s="4" t="s"/>
-      <c r="D3" s="4" t="s"/>
-      <c r="E3" s="4" t="s"/>
-      <c r="F3" s="2" t="s"/>
-      <c r="G3" s="2" t="s"/>
-      <c r="H3" s="2" t="s"/>
-      <c r="I3" s="2" t="s"/>
-    </row>
-    <row r="4" customHeight="1" ht="30">
-      <c r="A4" s="2" t="s"/>
-      <c r="B4" s="5" t="s">
+      <c r="H3" s="4" t="s"/>
+      <c r="I3" s="4" t="s"/>
+    </row>
+    <row r="4" customHeight="1" ht="31">
+      <c r="A4" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="5" t="s"/>
-      <c r="D4" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="E4" s="5" t="s"/>
-      <c r="F4" s="5" t="s"/>
-      <c r="G4" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="H4" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="I4" s="5" t="s"/>
-    </row>
-    <row r="5" customHeight="1" ht="30">
-      <c r="A5" s="2" t="s"/>
-      <c r="B5" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="C5" s="5" t="s"/>
-      <c r="D5" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="E5" s="5" t="s"/>
-      <c r="F5" s="5" t="s"/>
-      <c r="G5" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="H5" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="I5" s="5" t="s"/>
-    </row>
-    <row r="6" customHeight="1" ht="30">
+      <c r="B4" s="4" t="s"/>
+      <c r="C4" s="4" t="s"/>
+      <c r="D4" s="4" t="s"/>
+      <c r="E4" s="4" t="s"/>
+      <c r="F4" s="4" t="s"/>
+      <c r="G4" s="4" t="s"/>
+      <c r="H4" s="4" t="s"/>
+      <c r="I4" s="4" t="s"/>
+    </row>
+    <row r="5" customHeight="1" ht="29">
+      <c r="A5" s="4" t="s"/>
+      <c r="B5" s="4" t="s"/>
+      <c r="C5" s="4" t="s"/>
+      <c r="D5" s="4" t="s"/>
+      <c r="E5" s="4" t="s"/>
+      <c r="F5" s="4" t="s"/>
+      <c r="G5" s="2" t="s"/>
+      <c r="H5" s="2" t="s"/>
+      <c r="I5" s="2" t="s"/>
+    </row>
+    <row r="6" customHeight="1" ht="20">
       <c r="A6" s="2" t="s"/>
       <c r="B6" s="5" t="s">
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="C6" s="5" t="s"/>
       <c r="D6" s="5" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="E6" s="5" t="s"/>
-      <c r="F6" s="5" t="s"/>
-      <c r="G6" s="5" t="s">
-        <v>13</v>
-      </c>
+      <c r="F6" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="G6" s="5" t="s"/>
       <c r="H6" s="5" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="I6" s="5" t="s"/>
     </row>
-    <row r="7" customHeight="1" ht="30">
+    <row r="7" customHeight="1" ht="20">
       <c r="A7" s="2" t="s"/>
       <c r="B7" s="5" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C7" s="5" t="s"/>
       <c r="D7" s="5" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E7" s="5" t="s"/>
-      <c r="F7" s="5" t="s"/>
-      <c r="G7" s="5" t="s">
-        <v>9</v>
-      </c>
+      <c r="F7" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="G7" s="5" t="s"/>
       <c r="H7" s="5" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="I7" s="5" t="s"/>
     </row>
-    <row r="8" customHeight="1" ht="30">
+    <row r="8" customHeight="1" ht="20">
       <c r="A8" s="2" t="s"/>
       <c r="B8" s="5" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C8" s="5" t="s"/>
       <c r="D8" s="5" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E8" s="5" t="s"/>
-      <c r="F8" s="5" t="s"/>
-      <c r="G8" s="5" t="s">
-        <v>13</v>
-      </c>
+      <c r="F8" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="G8" s="5" t="s"/>
       <c r="H8" s="5" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="I8" s="5" t="s"/>
     </row>
-    <row r="9" customHeight="1" ht="30">
+    <row r="9" customHeight="1" ht="20">
       <c r="A9" s="2" t="s"/>
       <c r="B9" s="5" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C9" s="5" t="s"/>
       <c r="D9" s="5" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E9" s="5" t="s"/>
-      <c r="F9" s="5" t="s"/>
-      <c r="G9" s="5" t="s">
-        <v>9</v>
-      </c>
+      <c r="F9" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="G9" s="5" t="s"/>
       <c r="H9" s="5" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="I9" s="5" t="s"/>
     </row>
-    <row r="10" customHeight="1" ht="30">
+    <row r="10" customHeight="1" ht="20">
       <c r="A10" s="2" t="s"/>
       <c r="B10" s="5" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C10" s="5" t="s"/>
       <c r="D10" s="5" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E10" s="5" t="s"/>
-      <c r="F10" s="5" t="s"/>
-      <c r="G10" s="5" t="s">
-        <v>13</v>
-      </c>
+      <c r="F10" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="G10" s="5" t="s"/>
       <c r="H10" s="5" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="I10" s="5" t="s"/>
     </row>
-    <row r="11" customHeight="1" ht="30">
+    <row r="11" customHeight="1" ht="20">
       <c r="A11" s="2" t="s"/>
       <c r="B11" s="5" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C11" s="5" t="s"/>
       <c r="D11" s="5" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E11" s="5" t="s"/>
-      <c r="F11" s="5" t="s"/>
-      <c r="G11" s="5" t="s">
-        <v>9</v>
-      </c>
+      <c r="F11" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="G11" s="5" t="s"/>
       <c r="H11" s="5" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="I11" s="5" t="s"/>
     </row>
-    <row r="12" customHeight="1" ht="30">
+    <row r="12" customHeight="1" ht="20">
       <c r="A12" s="2" t="s"/>
       <c r="B12" s="5" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C12" s="5" t="s"/>
       <c r="D12" s="5" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E12" s="5" t="s"/>
-      <c r="F12" s="5" t="s"/>
-      <c r="G12" s="5" t="s">
-        <v>13</v>
-      </c>
+      <c r="F12" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="G12" s="5" t="s"/>
       <c r="H12" s="5" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="I12" s="5" t="s"/>
     </row>
-    <row r="13" customHeight="1" ht="30">
+    <row r="13" customHeight="1" ht="20">
       <c r="A13" s="2" t="s"/>
       <c r="B13" s="5" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C13" s="5" t="s"/>
       <c r="D13" s="5" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E13" s="5" t="s"/>
-      <c r="F13" s="5" t="s"/>
-      <c r="G13" s="5" t="s">
-        <v>9</v>
-      </c>
+      <c r="F13" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="G13" s="5" t="s"/>
       <c r="H13" s="5" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="I13" s="5" t="s"/>
     </row>
-    <row r="14" customHeight="1" ht="30">
+    <row r="14" customHeight="1" ht="20">
       <c r="A14" s="2" t="s"/>
       <c r="B14" s="5" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C14" s="5" t="s"/>
       <c r="D14" s="5" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E14" s="5" t="s"/>
-      <c r="F14" s="5" t="s"/>
-      <c r="G14" s="5" t="s">
-        <v>13</v>
-      </c>
+      <c r="F14" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="G14" s="5" t="s"/>
       <c r="H14" s="5" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="I14" s="5" t="s"/>
     </row>
-    <row r="15" customHeight="1" ht="30">
+    <row r="15" customHeight="1" ht="20">
       <c r="A15" s="2" t="s"/>
       <c r="B15" s="5" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C15" s="5" t="s"/>
       <c r="D15" s="5" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E15" s="5" t="s"/>
-      <c r="F15" s="5" t="s"/>
-      <c r="G15" s="5" t="s">
-        <v>9</v>
-      </c>
+      <c r="F15" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="G15" s="5" t="s"/>
       <c r="H15" s="5" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="I15" s="5" t="s"/>
     </row>
-    <row r="16" customHeight="1" ht="30">
+    <row r="16" customHeight="1" ht="20">
       <c r="A16" s="2" t="s"/>
       <c r="B16" s="5" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C16" s="5" t="s"/>
       <c r="D16" s="5" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E16" s="5" t="s"/>
-      <c r="F16" s="5" t="s"/>
-      <c r="G16" s="5" t="s">
-        <v>13</v>
-      </c>
+      <c r="F16" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="G16" s="5" t="s"/>
       <c r="H16" s="5" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="I16" s="5" t="s"/>
     </row>
-    <row r="17" customHeight="1" ht="30">
+    <row r="17" customHeight="1" ht="20">
       <c r="A17" s="2" t="s"/>
       <c r="B17" s="5" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C17" s="5" t="s"/>
       <c r="D17" s="5" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E17" s="5" t="s"/>
-      <c r="F17" s="5" t="s"/>
-      <c r="G17" s="5" t="s">
-        <v>9</v>
-      </c>
+      <c r="F17" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="G17" s="5" t="s"/>
       <c r="H17" s="5" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="I17" s="5" t="s"/>
     </row>
-    <row r="18" customHeight="1" ht="30">
+    <row r="18" customHeight="1" ht="20">
       <c r="A18" s="2" t="s"/>
       <c r="B18" s="5" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C18" s="5" t="s"/>
       <c r="D18" s="5" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E18" s="5" t="s"/>
-      <c r="F18" s="5" t="s"/>
-      <c r="G18" s="5" t="s">
-        <v>13</v>
-      </c>
+      <c r="F18" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="G18" s="5" t="s"/>
       <c r="H18" s="5" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="I18" s="5" t="s"/>
     </row>
-    <row r="19" customHeight="1" ht="30">
+    <row r="19" customHeight="1" ht="20">
       <c r="A19" s="2" t="s"/>
       <c r="B19" s="5" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C19" s="5" t="s"/>
       <c r="D19" s="5" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E19" s="5" t="s"/>
-      <c r="F19" s="5" t="s"/>
-      <c r="G19" s="5" t="s">
-        <v>9</v>
-      </c>
+      <c r="F19" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="G19" s="5" t="s"/>
       <c r="H19" s="5" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="I19" s="5" t="s"/>
     </row>
-    <row r="20" customHeight="1" ht="30">
+    <row r="20" customHeight="1" ht="20">
       <c r="A20" s="2" t="s"/>
       <c r="B20" s="5" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C20" s="5" t="s"/>
       <c r="D20" s="5" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E20" s="5" t="s"/>
-      <c r="F20" s="5" t="s"/>
-      <c r="G20" s="5" t="s">
-        <v>13</v>
-      </c>
+      <c r="F20" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="G20" s="5" t="s"/>
       <c r="H20" s="5" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="I20" s="5" t="s"/>
     </row>
-    <row r="21" customHeight="1" ht="30">
+    <row r="21" customHeight="1" ht="20">
       <c r="A21" s="2" t="s"/>
       <c r="B21" s="5" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C21" s="5" t="s"/>
       <c r="D21" s="5" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E21" s="5" t="s"/>
-      <c r="F21" s="5" t="s"/>
-      <c r="G21" s="5" t="s">
-        <v>9</v>
-      </c>
+      <c r="F21" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="G21" s="5" t="s"/>
       <c r="H21" s="5" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="I21" s="5" t="s"/>
     </row>
-    <row r="22" customHeight="1" ht="30">
+    <row r="22" customHeight="1" ht="20">
       <c r="A22" s="2" t="s"/>
       <c r="B22" s="5" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C22" s="5" t="s"/>
       <c r="D22" s="5" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E22" s="5" t="s"/>
-      <c r="F22" s="5" t="s"/>
-      <c r="G22" s="5" t="s">
-        <v>13</v>
-      </c>
+      <c r="F22" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="G22" s="5" t="s"/>
       <c r="H22" s="5" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="I22" s="5" t="s"/>
     </row>
-    <row r="23" customHeight="1" ht="30">
+    <row r="23" customHeight="1" ht="20">
       <c r="A23" s="2" t="s"/>
       <c r="B23" s="5" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C23" s="5" t="s"/>
       <c r="D23" s="5" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E23" s="5" t="s"/>
-      <c r="F23" s="5" t="s"/>
-      <c r="G23" s="5" t="s">
-        <v>9</v>
-      </c>
+      <c r="F23" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="G23" s="5" t="s"/>
       <c r="H23" s="5" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="I23" s="5" t="s"/>
     </row>
-    <row r="24" customHeight="1" ht="30">
+    <row r="24" customHeight="1" ht="20">
       <c r="A24" s="2" t="s"/>
       <c r="B24" s="5" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C24" s="5" t="s"/>
       <c r="D24" s="5" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E24" s="5" t="s"/>
-      <c r="F24" s="5" t="s"/>
-      <c r="G24" s="5" t="s">
-        <v>13</v>
-      </c>
+      <c r="F24" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="G24" s="5" t="s"/>
       <c r="H24" s="5" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="I24" s="5" t="s"/>
     </row>
-    <row r="25" customHeight="1" ht="30">
+    <row r="25" customHeight="1" ht="20">
       <c r="A25" s="2" t="s"/>
       <c r="B25" s="5" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C25" s="5" t="s"/>
       <c r="D25" s="5" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E25" s="5" t="s"/>
-      <c r="F25" s="5" t="s"/>
-      <c r="G25" s="5" t="s">
-        <v>9</v>
-      </c>
+      <c r="F25" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="G25" s="5" t="s"/>
       <c r="H25" s="5" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="I25" s="5" t="s"/>
     </row>
-    <row r="26" customHeight="1" ht="30">
+    <row r="26" customHeight="1" ht="20">
       <c r="A26" s="2" t="s"/>
       <c r="B26" s="5" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C26" s="5" t="s"/>
       <c r="D26" s="5" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E26" s="5" t="s"/>
-      <c r="F26" s="5" t="s"/>
-      <c r="G26" s="5" t="s">
-        <v>13</v>
-      </c>
+      <c r="F26" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="G26" s="5" t="s"/>
       <c r="H26" s="5" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="I26" s="5" t="s"/>
     </row>
-    <row r="27" customHeight="1" ht="30">
+    <row r="27" customHeight="1" ht="20">
       <c r="A27" s="2" t="s"/>
       <c r="B27" s="5" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C27" s="5" t="s"/>
       <c r="D27" s="5" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E27" s="5" t="s"/>
-      <c r="F27" s="5" t="s"/>
-      <c r="G27" s="5" t="s">
-        <v>9</v>
-      </c>
+      <c r="F27" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="G27" s="5" t="s"/>
       <c r="H27" s="5" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="I27" s="5" t="s"/>
     </row>
-    <row r="28" customHeight="1" ht="30">
+    <row r="28" customHeight="1" ht="20">
       <c r="A28" s="2" t="s"/>
       <c r="B28" s="5" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C28" s="5" t="s"/>
       <c r="D28" s="5" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E28" s="5" t="s"/>
-      <c r="F28" s="5" t="s"/>
-      <c r="G28" s="5" t="s">
-        <v>13</v>
-      </c>
+      <c r="F28" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="G28" s="5" t="s"/>
       <c r="H28" s="5" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="I28" s="5" t="s"/>
     </row>
-    <row r="29" customHeight="1" ht="30">
+    <row r="29" customHeight="1" ht="20">
       <c r="A29" s="2" t="s"/>
       <c r="B29" s="5" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C29" s="5" t="s"/>
       <c r="D29" s="5" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E29" s="5" t="s"/>
-      <c r="F29" s="5" t="s"/>
-      <c r="G29" s="5" t="s">
-        <v>9</v>
-      </c>
+      <c r="F29" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="G29" s="5" t="s"/>
       <c r="H29" s="5" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="I29" s="5" t="s"/>
     </row>
-    <row r="30" customHeight="1" ht="30">
+    <row r="30" customHeight="1" ht="20">
       <c r="A30" s="2" t="s"/>
       <c r="B30" s="5" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C30" s="5" t="s"/>
       <c r="D30" s="5" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E30" s="5" t="s"/>
-      <c r="F30" s="5" t="s"/>
-      <c r="G30" s="5" t="s">
-        <v>13</v>
-      </c>
+      <c r="F30" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="G30" s="5" t="s"/>
       <c r="H30" s="5" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="I30" s="5" t="s"/>
     </row>
-    <row r="31" customHeight="1" ht="30">
+    <row r="31" customHeight="1" ht="20">
       <c r="A31" s="2" t="s"/>
       <c r="B31" s="5" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C31" s="5" t="s"/>
       <c r="D31" s="5" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E31" s="5" t="s"/>
-      <c r="F31" s="5" t="s"/>
-      <c r="G31" s="5" t="s">
-        <v>9</v>
-      </c>
+      <c r="F31" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="G31" s="5" t="s"/>
       <c r="H31" s="5" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="I31" s="5" t="s"/>
     </row>
-    <row r="32" customHeight="1" ht="30">
+    <row r="32" customHeight="1" ht="20">
       <c r="A32" s="2" t="s"/>
       <c r="B32" s="5" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C32" s="5" t="s"/>
       <c r="D32" s="5" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E32" s="5" t="s"/>
-      <c r="F32" s="5" t="s"/>
-      <c r="G32" s="5" t="s">
-        <v>13</v>
-      </c>
+      <c r="F32" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="G32" s="5" t="s"/>
       <c r="H32" s="5" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="I32" s="5" t="s"/>
     </row>
-    <row r="33" customHeight="1" ht="30">
+    <row r="33" customHeight="1" ht="20">
       <c r="A33" s="2" t="s"/>
       <c r="B33" s="5" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C33" s="5" t="s"/>
       <c r="D33" s="5" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E33" s="5" t="s"/>
-      <c r="F33" s="5" t="s"/>
-      <c r="G33" s="5" t="s">
-        <v>9</v>
-      </c>
+      <c r="F33" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="G33" s="5" t="s"/>
       <c r="H33" s="5" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="I33" s="5" t="s"/>
     </row>
-    <row r="34" customHeight="1" ht="30">
+    <row r="34" customHeight="1" ht="20">
       <c r="A34" s="2" t="s"/>
       <c r="B34" s="5" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C34" s="5" t="s"/>
       <c r="D34" s="5" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E34" s="5" t="s"/>
-      <c r="F34" s="5" t="s"/>
-      <c r="G34" s="5" t="s">
-        <v>13</v>
-      </c>
+      <c r="F34" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="G34" s="5" t="s"/>
       <c r="H34" s="5" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="I34" s="5" t="s"/>
     </row>
-    <row r="35" customHeight="1" ht="30">
+    <row r="35" customHeight="1" ht="20">
       <c r="A35" s="2" t="s"/>
       <c r="B35" s="5" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C35" s="5" t="s"/>
       <c r="D35" s="5" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E35" s="5" t="s"/>
-      <c r="F35" s="5" t="s"/>
-      <c r="G35" s="5" t="s">
-        <v>9</v>
-      </c>
+      <c r="F35" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="G35" s="5" t="s"/>
       <c r="H35" s="5" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="I35" s="5" t="s"/>
     </row>
-    <row r="36" customHeight="1" ht="30">
+    <row r="36" customHeight="1" ht="20">
       <c r="A36" s="2" t="s"/>
       <c r="B36" s="5" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C36" s="5" t="s"/>
       <c r="D36" s="5" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E36" s="5" t="s"/>
-      <c r="F36" s="5" t="s"/>
-      <c r="G36" s="5" t="s">
-        <v>13</v>
-      </c>
+      <c r="F36" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="G36" s="5" t="s"/>
       <c r="H36" s="5" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="I36" s="5" t="s"/>
     </row>
-    <row r="37" customHeight="1" ht="30">
+    <row r="37" customHeight="1" ht="20">
       <c r="A37" s="2" t="s"/>
       <c r="B37" s="5" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C37" s="5" t="s"/>
       <c r="D37" s="5" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E37" s="5" t="s"/>
-      <c r="F37" s="5" t="s"/>
-      <c r="G37" s="5" t="s">
-        <v>9</v>
-      </c>
+      <c r="F37" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="G37" s="5" t="s"/>
       <c r="H37" s="5" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="I37" s="5" t="s"/>
     </row>
-    <row r="38" customHeight="1" ht="30">
+    <row r="38" customHeight="1" ht="20">
       <c r="A38" s="2" t="s"/>
       <c r="B38" s="5" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C38" s="5" t="s"/>
       <c r="D38" s="5" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E38" s="5" t="s"/>
-      <c r="F38" s="5" t="s"/>
-      <c r="G38" s="5" t="s">
-        <v>13</v>
-      </c>
+      <c r="F38" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="G38" s="5" t="s"/>
       <c r="H38" s="5" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="I38" s="5" t="s"/>
     </row>
-    <row r="39" customHeight="1" ht="30">
+    <row r="39" customHeight="1" ht="20">
       <c r="A39" s="2" t="s"/>
       <c r="B39" s="5" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C39" s="5" t="s"/>
       <c r="D39" s="5" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E39" s="5" t="s"/>
-      <c r="F39" s="5" t="s"/>
-      <c r="G39" s="5" t="s">
-        <v>9</v>
-      </c>
+      <c r="F39" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="G39" s="5" t="s"/>
       <c r="H39" s="5" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="I39" s="5" t="s"/>
     </row>
-    <row r="40" customHeight="1" ht="30">
+    <row r="40" customHeight="1" ht="20">
       <c r="A40" s="2" t="s"/>
       <c r="B40" s="5" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C40" s="5" t="s"/>
       <c r="D40" s="5" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E40" s="5" t="s"/>
-      <c r="F40" s="5" t="s"/>
-      <c r="G40" s="5" t="s">
-        <v>13</v>
-      </c>
+      <c r="F40" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="G40" s="5" t="s"/>
       <c r="H40" s="5" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="I40" s="5" t="s"/>
     </row>
-    <row r="41" customHeight="1" ht="30">
+    <row r="41" customHeight="1" ht="20">
       <c r="A41" s="2" t="s"/>
       <c r="B41" s="5" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C41" s="5" t="s"/>
       <c r="D41" s="5" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E41" s="5" t="s"/>
-      <c r="F41" s="5" t="s"/>
-      <c r="G41" s="5" t="s">
-        <v>9</v>
-      </c>
+      <c r="F41" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="G41" s="5" t="s"/>
       <c r="H41" s="5" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="I41" s="5" t="s"/>
     </row>
-    <row r="42" customHeight="1" ht="30">
+    <row r="42" customHeight="1" ht="20">
       <c r="A42" s="2" t="s"/>
       <c r="B42" s="5" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C42" s="5" t="s"/>
       <c r="D42" s="5" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E42" s="5" t="s"/>
-      <c r="F42" s="5" t="s"/>
-      <c r="G42" s="5" t="s">
-        <v>13</v>
-      </c>
+      <c r="F42" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="G42" s="5" t="s"/>
       <c r="H42" s="5" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="I42" s="5" t="s"/>
     </row>
-    <row r="43" customHeight="1" ht="30">
+    <row r="43" customHeight="1" ht="20">
       <c r="A43" s="2" t="s"/>
       <c r="B43" s="5" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C43" s="5" t="s"/>
       <c r="D43" s="5" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E43" s="5" t="s"/>
-      <c r="F43" s="5" t="s"/>
-      <c r="G43" s="5" t="s">
-        <v>9</v>
-      </c>
+      <c r="F43" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="G43" s="5" t="s"/>
       <c r="H43" s="5" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="I43" s="5" t="s"/>
     </row>
-    <row r="44" customHeight="1" ht="30">
+    <row r="44" customHeight="1" ht="20">
       <c r="A44" s="2" t="s"/>
       <c r="B44" s="5" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C44" s="5" t="s"/>
       <c r="D44" s="5" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E44" s="5" t="s"/>
-      <c r="F44" s="5" t="s"/>
-      <c r="G44" s="5" t="s">
-        <v>13</v>
-      </c>
+      <c r="F44" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="G44" s="5" t="s"/>
       <c r="H44" s="5" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="I44" s="5" t="s"/>
     </row>
-    <row r="45" customHeight="1" ht="30">
+    <row r="45" customHeight="1" ht="20">
       <c r="A45" s="2" t="s"/>
       <c r="B45" s="5" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C45" s="5" t="s"/>
       <c r="D45" s="5" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E45" s="5" t="s"/>
-      <c r="F45" s="5" t="s"/>
-      <c r="G45" s="5" t="s">
-        <v>9</v>
-      </c>
+      <c r="F45" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="G45" s="5" t="s"/>
       <c r="H45" s="5" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="I45" s="5" t="s"/>
     </row>
-    <row r="46" customHeight="1" ht="30">
+    <row r="46" customHeight="1" ht="20">
       <c r="A46" s="2" t="s"/>
       <c r="B46" s="5" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C46" s="5" t="s"/>
       <c r="D46" s="5" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E46" s="5" t="s"/>
-      <c r="F46" s="5" t="s"/>
-      <c r="G46" s="5" t="s">
-        <v>13</v>
-      </c>
+      <c r="F46" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="G46" s="5" t="s"/>
       <c r="H46" s="5" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="I46" s="5" t="s"/>
     </row>
-    <row r="47" customHeight="1" ht="30">
+    <row r="47" customHeight="1" ht="20">
       <c r="A47" s="2" t="s"/>
       <c r="B47" s="5" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C47" s="5" t="s"/>
       <c r="D47" s="5" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E47" s="5" t="s"/>
-      <c r="F47" s="5" t="s"/>
-      <c r="G47" s="5" t="s">
-        <v>9</v>
-      </c>
+      <c r="F47" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="G47" s="5" t="s"/>
       <c r="H47" s="5" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="I47" s="5" t="s"/>
     </row>
-    <row r="48" customHeight="1" ht="30">
+    <row r="48" customHeight="1" ht="20">
       <c r="A48" s="2" t="s"/>
       <c r="B48" s="5" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C48" s="5" t="s"/>
       <c r="D48" s="5" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E48" s="5" t="s"/>
-      <c r="F48" s="5" t="s"/>
-      <c r="G48" s="5" t="s">
-        <v>13</v>
-      </c>
+      <c r="F48" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="G48" s="5" t="s"/>
       <c r="H48" s="5" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="I48" s="5" t="s"/>
     </row>
-    <row r="49" customHeight="1" ht="30">
+    <row r="49" customHeight="1" ht="20">
       <c r="A49" s="2" t="s"/>
       <c r="B49" s="5" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C49" s="5" t="s"/>
       <c r="D49" s="5" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E49" s="5" t="s"/>
-      <c r="F49" s="5" t="s"/>
-      <c r="G49" s="5" t="s">
-        <v>9</v>
-      </c>
+      <c r="F49" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="G49" s="5" t="s"/>
       <c r="H49" s="5" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="I49" s="5" t="s"/>
     </row>
-    <row r="50" customHeight="1" ht="30">
+    <row r="50" customHeight="1" ht="20">
       <c r="A50" s="2" t="s"/>
       <c r="B50" s="5" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C50" s="5" t="s"/>
       <c r="D50" s="5" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E50" s="5" t="s"/>
-      <c r="F50" s="5" t="s"/>
-      <c r="G50" s="5" t="s">
-        <v>13</v>
-      </c>
+      <c r="F50" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="G50" s="5" t="s"/>
       <c r="H50" s="5" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="I50" s="5" t="s"/>
     </row>
-    <row r="51" customHeight="1" ht="30">
+    <row r="51" customHeight="1" ht="20">
       <c r="A51" s="2" t="s"/>
       <c r="B51" s="5" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C51" s="5" t="s"/>
       <c r="D51" s="5" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E51" s="5" t="s"/>
-      <c r="F51" s="5" t="s"/>
-      <c r="G51" s="5" t="s">
-        <v>9</v>
-      </c>
+      <c r="F51" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="G51" s="5" t="s"/>
       <c r="H51" s="5" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="I51" s="5" t="s"/>
     </row>
-    <row r="52" customHeight="1" ht="30">
+    <row r="52" customHeight="1" ht="20">
       <c r="A52" s="2" t="s"/>
       <c r="B52" s="5" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C52" s="5" t="s"/>
       <c r="D52" s="5" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E52" s="5" t="s"/>
-      <c r="F52" s="5" t="s"/>
-      <c r="G52" s="5" t="s">
-        <v>13</v>
-      </c>
+      <c r="F52" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="G52" s="5" t="s"/>
       <c r="H52" s="5" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="I52" s="5" t="s"/>
     </row>
-    <row r="53" customHeight="1" ht="30">
+    <row r="53" customHeight="1" ht="20">
       <c r="A53" s="2" t="s"/>
       <c r="B53" s="5" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C53" s="5" t="s"/>
       <c r="D53" s="5" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E53" s="5" t="s"/>
-      <c r="F53" s="5" t="s"/>
-      <c r="G53" s="5" t="s">
-        <v>9</v>
-      </c>
+      <c r="F53" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="G53" s="5" t="s"/>
       <c r="H53" s="5" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="I53" s="5" t="s"/>
     </row>
-    <row r="54" customHeight="1" ht="30">
+    <row r="54" customHeight="1" ht="20">
       <c r="A54" s="2" t="s"/>
       <c r="B54" s="5" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C54" s="5" t="s"/>
       <c r="D54" s="5" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E54" s="5" t="s"/>
-      <c r="F54" s="5" t="s"/>
-      <c r="G54" s="5" t="s">
-        <v>13</v>
-      </c>
+      <c r="F54" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="G54" s="5" t="s"/>
       <c r="H54" s="5" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="I54" s="5" t="s"/>
     </row>
-    <row r="55" customHeight="1" ht="30">
+    <row r="55" customHeight="1" ht="20">
       <c r="A55" s="2" t="s"/>
       <c r="B55" s="5" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C55" s="5" t="s"/>
       <c r="D55" s="5" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E55" s="5" t="s"/>
-      <c r="F55" s="5" t="s"/>
-      <c r="G55" s="5" t="s">
-        <v>9</v>
-      </c>
+      <c r="F55" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="G55" s="5" t="s"/>
       <c r="H55" s="5" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="I55" s="5" t="s"/>
     </row>
-    <row r="56" customHeight="1" ht="30">
+    <row r="56" customHeight="1" ht="20">
       <c r="A56" s="2" t="s"/>
       <c r="B56" s="5" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C56" s="5" t="s"/>
       <c r="D56" s="5" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E56" s="5" t="s"/>
-      <c r="F56" s="5" t="s"/>
-      <c r="G56" s="5" t="s">
-        <v>13</v>
-      </c>
+      <c r="F56" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="G56" s="5" t="s"/>
       <c r="H56" s="5" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="I56" s="5" t="s"/>
     </row>
-    <row r="57" customHeight="1" ht="30">
+    <row r="57" customHeight="1" ht="20">
       <c r="A57" s="2" t="s"/>
       <c r="B57" s="5" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C57" s="5" t="s"/>
       <c r="D57" s="5" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E57" s="5" t="s"/>
-      <c r="F57" s="5" t="s"/>
-      <c r="G57" s="5" t="s">
-        <v>9</v>
-      </c>
+      <c r="F57" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="G57" s="5" t="s"/>
       <c r="H57" s="5" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="I57" s="5" t="s"/>
     </row>
-    <row r="58" customHeight="1" ht="30">
+    <row r="58" customHeight="1" ht="20">
       <c r="A58" s="2" t="s"/>
       <c r="B58" s="5" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C58" s="5" t="s"/>
       <c r="D58" s="5" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E58" s="5" t="s"/>
-      <c r="F58" s="5" t="s"/>
-      <c r="G58" s="5" t="s">
-        <v>13</v>
-      </c>
+      <c r="F58" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="G58" s="5" t="s"/>
       <c r="H58" s="5" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="I58" s="5" t="s"/>
     </row>
-    <row r="59" customHeight="1" ht="30">
+    <row r="59" customHeight="1" ht="20">
       <c r="A59" s="2" t="s"/>
       <c r="B59" s="5" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C59" s="5" t="s"/>
       <c r="D59" s="5" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E59" s="5" t="s"/>
-      <c r="F59" s="5" t="s"/>
-      <c r="G59" s="5" t="s">
-        <v>9</v>
-      </c>
+      <c r="F59" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="G59" s="5" t="s"/>
       <c r="H59" s="5" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="I59" s="5" t="s"/>
     </row>
-    <row r="60" customHeight="1" ht="30">
+    <row r="60" customHeight="1" ht="20">
       <c r="A60" s="2" t="s"/>
       <c r="B60" s="5" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C60" s="5" t="s"/>
       <c r="D60" s="5" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E60" s="5" t="s"/>
-      <c r="F60" s="5" t="s"/>
-      <c r="G60" s="5" t="s">
-        <v>13</v>
-      </c>
+      <c r="F60" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="G60" s="5" t="s"/>
       <c r="H60" s="5" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="I60" s="5" t="s"/>
     </row>
-    <row r="61" customHeight="1" ht="31">
+    <row r="61" customHeight="1" ht="20">
       <c r="A61" s="2" t="s"/>
-      <c r="B61" s="2" t="s"/>
-      <c r="C61" s="2" t="s"/>
-      <c r="D61" s="2" t="s"/>
-      <c r="E61" s="2" t="s"/>
-      <c r="F61" s="2" t="s"/>
-      <c r="G61" s="2" t="s"/>
-      <c r="H61" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="I61" s="6" t="s"/>
+      <c r="B61" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C61" s="5" t="s"/>
+      <c r="D61" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E61" s="5" t="s"/>
+      <c r="F61" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="G61" s="5" t="s"/>
+      <c r="H61" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="I61" s="5" t="s"/>
+    </row>
+    <row r="62" customHeight="1" ht="20">
+      <c r="A62" s="2" t="s"/>
+      <c r="B62" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C62" s="5" t="s"/>
+      <c r="D62" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E62" s="5" t="s"/>
+      <c r="F62" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="G62" s="5" t="s"/>
+      <c r="H62" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="I62" s="5" t="s"/>
+    </row>
+    <row r="63" customHeight="1" ht="31">
+      <c r="A63" s="2" t="s"/>
+      <c r="B63" s="2" t="s"/>
+      <c r="C63" s="2" t="s"/>
+      <c r="D63" s="2" t="s"/>
+      <c r="E63" s="2" t="s"/>
+      <c r="F63" s="2" t="s"/>
+      <c r="G63" s="2" t="s"/>
+      <c r="H63" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="I63" s="6" t="s"/>
     </row>
   </sheetData>
   <mergeCells>
     <mergeCell ref="A1:D1"/>
     <mergeCell ref="C2:H2"/>
-    <mergeCell ref="A3:E3"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="D4:F4"/>
-    <mergeCell ref="H4:I4"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="D5:F5"/>
-    <mergeCell ref="H5:I5"/>
+    <mergeCell ref="G3:I4"/>
+    <mergeCell ref="A4:F5"/>
     <mergeCell ref="B6:C6"/>
-    <mergeCell ref="D6:F6"/>
+    <mergeCell ref="D6:E6"/>
+    <mergeCell ref="F6:G6"/>
     <mergeCell ref="H6:I6"/>
     <mergeCell ref="B7:C7"/>
-    <mergeCell ref="D7:F7"/>
+    <mergeCell ref="D7:E7"/>
+    <mergeCell ref="F7:G7"/>
     <mergeCell ref="H7:I7"/>
     <mergeCell ref="B8:C8"/>
-    <mergeCell ref="D8:F8"/>
+    <mergeCell ref="D8:E8"/>
+    <mergeCell ref="F8:G8"/>
     <mergeCell ref="H8:I8"/>
     <mergeCell ref="B9:C9"/>
-    <mergeCell ref="D9:F9"/>
+    <mergeCell ref="D9:E9"/>
+    <mergeCell ref="F9:G9"/>
     <mergeCell ref="H9:I9"/>
     <mergeCell ref="B10:C10"/>
-    <mergeCell ref="D10:F10"/>
+    <mergeCell ref="D10:E10"/>
+    <mergeCell ref="F10:G10"/>
     <mergeCell ref="H10:I10"/>
     <mergeCell ref="B11:C11"/>
-    <mergeCell ref="D11:F11"/>
+    <mergeCell ref="D11:E11"/>
+    <mergeCell ref="F11:G11"/>
     <mergeCell ref="H11:I11"/>
     <mergeCell ref="B12:C12"/>
-    <mergeCell ref="D12:F12"/>
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="F12:G12"/>
     <mergeCell ref="H12:I12"/>
     <mergeCell ref="B13:C13"/>
-    <mergeCell ref="D13:F13"/>
+    <mergeCell ref="D13:E13"/>
+    <mergeCell ref="F13:G13"/>
     <mergeCell ref="H13:I13"/>
     <mergeCell ref="B14:C14"/>
-    <mergeCell ref="D14:F14"/>
+    <mergeCell ref="D14:E14"/>
+    <mergeCell ref="F14:G14"/>
     <mergeCell ref="H14:I14"/>
     <mergeCell ref="B15:C15"/>
-    <mergeCell ref="D15:F15"/>
+    <mergeCell ref="D15:E15"/>
+    <mergeCell ref="F15:G15"/>
     <mergeCell ref="H15:I15"/>
     <mergeCell ref="B16:C16"/>
-    <mergeCell ref="D16:F16"/>
+    <mergeCell ref="D16:E16"/>
+    <mergeCell ref="F16:G16"/>
     <mergeCell ref="H16:I16"/>
     <mergeCell ref="B17:C17"/>
-    <mergeCell ref="D17:F17"/>
+    <mergeCell ref="D17:E17"/>
+    <mergeCell ref="F17:G17"/>
     <mergeCell ref="H17:I17"/>
     <mergeCell ref="B18:C18"/>
-    <mergeCell ref="D18:F18"/>
+    <mergeCell ref="D18:E18"/>
+    <mergeCell ref="F18:G18"/>
     <mergeCell ref="H18:I18"/>
     <mergeCell ref="B19:C19"/>
-    <mergeCell ref="D19:F19"/>
+    <mergeCell ref="D19:E19"/>
+    <mergeCell ref="F19:G19"/>
     <mergeCell ref="H19:I19"/>
     <mergeCell ref="B20:C20"/>
-    <mergeCell ref="D20:F20"/>
+    <mergeCell ref="D20:E20"/>
+    <mergeCell ref="F20:G20"/>
     <mergeCell ref="H20:I20"/>
     <mergeCell ref="B21:C21"/>
-    <mergeCell ref="D21:F21"/>
+    <mergeCell ref="D21:E21"/>
+    <mergeCell ref="F21:G21"/>
     <mergeCell ref="H21:I21"/>
     <mergeCell ref="B22:C22"/>
-    <mergeCell ref="D22:F22"/>
+    <mergeCell ref="D22:E22"/>
+    <mergeCell ref="F22:G22"/>
     <mergeCell ref="H22:I22"/>
     <mergeCell ref="B23:C23"/>
-    <mergeCell ref="D23:F23"/>
+    <mergeCell ref="D23:E23"/>
+    <mergeCell ref="F23:G23"/>
     <mergeCell ref="H23:I23"/>
     <mergeCell ref="B24:C24"/>
-    <mergeCell ref="D24:F24"/>
+    <mergeCell ref="D24:E24"/>
+    <mergeCell ref="F24:G24"/>
     <mergeCell ref="H24:I24"/>
     <mergeCell ref="B25:C25"/>
-    <mergeCell ref="D25:F25"/>
+    <mergeCell ref="D25:E25"/>
+    <mergeCell ref="F25:G25"/>
     <mergeCell ref="H25:I25"/>
     <mergeCell ref="B26:C26"/>
-    <mergeCell ref="D26:F26"/>
+    <mergeCell ref="D26:E26"/>
+    <mergeCell ref="F26:G26"/>
     <mergeCell ref="H26:I26"/>
     <mergeCell ref="B27:C27"/>
-    <mergeCell ref="D27:F27"/>
+    <mergeCell ref="D27:E27"/>
+    <mergeCell ref="F27:G27"/>
     <mergeCell ref="H27:I27"/>
     <mergeCell ref="B28:C28"/>
-    <mergeCell ref="D28:F28"/>
+    <mergeCell ref="D28:E28"/>
+    <mergeCell ref="F28:G28"/>
     <mergeCell ref="H28:I28"/>
     <mergeCell ref="B29:C29"/>
-    <mergeCell ref="D29:F29"/>
+    <mergeCell ref="D29:E29"/>
+    <mergeCell ref="F29:G29"/>
     <mergeCell ref="H29:I29"/>
     <mergeCell ref="B30:C30"/>
-    <mergeCell ref="D30:F30"/>
+    <mergeCell ref="D30:E30"/>
+    <mergeCell ref="F30:G30"/>
     <mergeCell ref="H30:I30"/>
     <mergeCell ref="B31:C31"/>
-    <mergeCell ref="D31:F31"/>
+    <mergeCell ref="D31:E31"/>
+    <mergeCell ref="F31:G31"/>
     <mergeCell ref="H31:I31"/>
     <mergeCell ref="B32:C32"/>
-    <mergeCell ref="D32:F32"/>
+    <mergeCell ref="D32:E32"/>
+    <mergeCell ref="F32:G32"/>
     <mergeCell ref="H32:I32"/>
     <mergeCell ref="B33:C33"/>
-    <mergeCell ref="D33:F33"/>
+    <mergeCell ref="D33:E33"/>
+    <mergeCell ref="F33:G33"/>
     <mergeCell ref="H33:I33"/>
     <mergeCell ref="B34:C34"/>
-    <mergeCell ref="D34:F34"/>
+    <mergeCell ref="D34:E34"/>
+    <mergeCell ref="F34:G34"/>
     <mergeCell ref="H34:I34"/>
     <mergeCell ref="B35:C35"/>
-    <mergeCell ref="D35:F35"/>
+    <mergeCell ref="D35:E35"/>
+    <mergeCell ref="F35:G35"/>
     <mergeCell ref="H35:I35"/>
     <mergeCell ref="B36:C36"/>
-    <mergeCell ref="D36:F36"/>
+    <mergeCell ref="D36:E36"/>
+    <mergeCell ref="F36:G36"/>
     <mergeCell ref="H36:I36"/>
     <mergeCell ref="B37:C37"/>
-    <mergeCell ref="D37:F37"/>
+    <mergeCell ref="D37:E37"/>
+    <mergeCell ref="F37:G37"/>
     <mergeCell ref="H37:I37"/>
     <mergeCell ref="B38:C38"/>
-    <mergeCell ref="D38:F38"/>
+    <mergeCell ref="D38:E38"/>
+    <mergeCell ref="F38:G38"/>
     <mergeCell ref="H38:I38"/>
     <mergeCell ref="B39:C39"/>
-    <mergeCell ref="D39:F39"/>
+    <mergeCell ref="D39:E39"/>
+    <mergeCell ref="F39:G39"/>
     <mergeCell ref="H39:I39"/>
     <mergeCell ref="B40:C40"/>
-    <mergeCell ref="D40:F40"/>
+    <mergeCell ref="D40:E40"/>
+    <mergeCell ref="F40:G40"/>
     <mergeCell ref="H40:I40"/>
     <mergeCell ref="B41:C41"/>
-    <mergeCell ref="D41:F41"/>
+    <mergeCell ref="D41:E41"/>
+    <mergeCell ref="F41:G41"/>
     <mergeCell ref="H41:I41"/>
     <mergeCell ref="B42:C42"/>
-    <mergeCell ref="D42:F42"/>
+    <mergeCell ref="D42:E42"/>
+    <mergeCell ref="F42:G42"/>
     <mergeCell ref="H42:I42"/>
     <mergeCell ref="B43:C43"/>
-    <mergeCell ref="D43:F43"/>
+    <mergeCell ref="D43:E43"/>
+    <mergeCell ref="F43:G43"/>
     <mergeCell ref="H43:I43"/>
     <mergeCell ref="B44:C44"/>
-    <mergeCell ref="D44:F44"/>
+    <mergeCell ref="D44:E44"/>
+    <mergeCell ref="F44:G44"/>
     <mergeCell ref="H44:I44"/>
     <mergeCell ref="B45:C45"/>
-    <mergeCell ref="D45:F45"/>
+    <mergeCell ref="D45:E45"/>
+    <mergeCell ref="F45:G45"/>
     <mergeCell ref="H45:I45"/>
     <mergeCell ref="B46:C46"/>
-    <mergeCell ref="D46:F46"/>
+    <mergeCell ref="D46:E46"/>
+    <mergeCell ref="F46:G46"/>
     <mergeCell ref="H46:I46"/>
     <mergeCell ref="B47:C47"/>
-    <mergeCell ref="D47:F47"/>
+    <mergeCell ref="D47:E47"/>
+    <mergeCell ref="F47:G47"/>
     <mergeCell ref="H47:I47"/>
     <mergeCell ref="B48:C48"/>
-    <mergeCell ref="D48:F48"/>
+    <mergeCell ref="D48:E48"/>
+    <mergeCell ref="F48:G48"/>
     <mergeCell ref="H48:I48"/>
     <mergeCell ref="B49:C49"/>
-    <mergeCell ref="D49:F49"/>
+    <mergeCell ref="D49:E49"/>
+    <mergeCell ref="F49:G49"/>
     <mergeCell ref="H49:I49"/>
     <mergeCell ref="B50:C50"/>
-    <mergeCell ref="D50:F50"/>
+    <mergeCell ref="D50:E50"/>
+    <mergeCell ref="F50:G50"/>
     <mergeCell ref="H50:I50"/>
     <mergeCell ref="B51:C51"/>
-    <mergeCell ref="D51:F51"/>
+    <mergeCell ref="D51:E51"/>
+    <mergeCell ref="F51:G51"/>
     <mergeCell ref="H51:I51"/>
     <mergeCell ref="B52:C52"/>
-    <mergeCell ref="D52:F52"/>
+    <mergeCell ref="D52:E52"/>
+    <mergeCell ref="F52:G52"/>
     <mergeCell ref="H52:I52"/>
     <mergeCell ref="B53:C53"/>
-    <mergeCell ref="D53:F53"/>
+    <mergeCell ref="D53:E53"/>
+    <mergeCell ref="F53:G53"/>
     <mergeCell ref="H53:I53"/>
     <mergeCell ref="B54:C54"/>
-    <mergeCell ref="D54:F54"/>
+    <mergeCell ref="D54:E54"/>
+    <mergeCell ref="F54:G54"/>
     <mergeCell ref="H54:I54"/>
     <mergeCell ref="B55:C55"/>
-    <mergeCell ref="D55:F55"/>
+    <mergeCell ref="D55:E55"/>
+    <mergeCell ref="F55:G55"/>
     <mergeCell ref="H55:I55"/>
     <mergeCell ref="B56:C56"/>
-    <mergeCell ref="D56:F56"/>
+    <mergeCell ref="D56:E56"/>
+    <mergeCell ref="F56:G56"/>
     <mergeCell ref="H56:I56"/>
     <mergeCell ref="B57:C57"/>
-    <mergeCell ref="D57:F57"/>
+    <mergeCell ref="D57:E57"/>
+    <mergeCell ref="F57:G57"/>
     <mergeCell ref="H57:I57"/>
     <mergeCell ref="B58:C58"/>
-    <mergeCell ref="D58:F58"/>
+    <mergeCell ref="D58:E58"/>
+    <mergeCell ref="F58:G58"/>
     <mergeCell ref="H58:I58"/>
     <mergeCell ref="B59:C59"/>
-    <mergeCell ref="D59:F59"/>
+    <mergeCell ref="D59:E59"/>
+    <mergeCell ref="F59:G59"/>
     <mergeCell ref="H59:I59"/>
     <mergeCell ref="B60:C60"/>
-    <mergeCell ref="D60:F60"/>
+    <mergeCell ref="D60:E60"/>
+    <mergeCell ref="F60:G60"/>
     <mergeCell ref="H60:I60"/>
+    <mergeCell ref="B61:C61"/>
+    <mergeCell ref="D61:E61"/>
+    <mergeCell ref="F61:G61"/>
     <mergeCell ref="H61:I61"/>
+    <mergeCell ref="B62:C62"/>
+    <mergeCell ref="D62:E62"/>
+    <mergeCell ref="F62:G62"/>
+    <mergeCell ref="H62:I62"/>
+    <mergeCell ref="H63:I63"/>
   </mergeCells>
   <pageMargins left="0.0" right="0.0" top="0.0" bottom="0.00" header="0.0" footer="0.0"/>
   <pageSetup orientation="portrait" paperSize="9"/>

</xml_diff>